<commit_message>
Trained the XGBoost models.
</commit_message>
<xml_diff>
--- a/model_analysis.xlsx
+++ b/model_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/31a3af44735637da/BWSI piPACT/piPACT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="11_F25DC773A252ABDACC1048834919455E5ADE58E8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E1D6725D-608C-4199-B852-54A492F333FE}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="11_F25DC773A252ABDACC1048834919455E5ADE58E8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1FA7BB63-D003-414C-801C-CAAC994B4011}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="41">
   <si>
     <t>Model</t>
   </si>
@@ -117,13 +117,37 @@
     <t>(Implemented with )</t>
   </si>
   <si>
-    <t>n_estimators=396, max_depth=5, min_child_weight=3, gamma=0., colsample_bytree=0.7, subsample=0.8, reg_alpha=4, reg_lamba=0</t>
-  </si>
-  <si>
     <t>n_estimators=37, max_depth=5, min_child_weight=1, gamma=0.1, colsample_bytree=0.01, subsample=0.8, reg_alpha=5, reg_lambda=0</t>
   </si>
   <si>
     <t>n_estimators=2139, max_depth=3, min_child_weight=3, gamma=0.1, colsample_bytree=0.01, subsample=0.2, reg_alpha=0.01, reg_lambda=0</t>
+  </si>
+  <si>
+    <t>n_estimators=3, max_depth=3, min_child_weight=1, gamma=0, colsample_bytree=0.01, subsample=0.1, reg_alpha=0, reg_lambda=0</t>
+  </si>
+  <si>
+    <t>n_estimators=396, max_depth=5, min_child_weight=3, gamma=0, colsample_bytree=0.7, subsample=0.8, reg_alpha=4, reg_lamba=0</t>
+  </si>
+  <si>
+    <t>n_neighbors=1381, metric='manhattan'</t>
+  </si>
+  <si>
+    <t>n_estimators=485, max_depth=3, min_child_weight=1, gamma=0, colsample_bytree=0.01, subsample=0.03, reg_alpha=0, reg_lambda=0</t>
+  </si>
+  <si>
+    <t>n_neighbors=1081, metric='manhattan'</t>
+  </si>
+  <si>
+    <t>n_estimators=2815, max_depth=4, min_child_weight=2, gamma=0.2, colsample_bytree=0.01, subsample=0.76, reg_alpha=0.01, reg_lambda=0</t>
+  </si>
+  <si>
+    <t>n_estimators=733, max_depth=4, min_child_weight=3, gamma=0.1, colsample_bytree=0.01, subsample=0.83, reg_alpha=0.01, reg_lambda=0</t>
+  </si>
+  <si>
+    <t>n_neighbors=19, metric='manhattan', n_components=2</t>
+  </si>
+  <si>
+    <t>n_estimators=2445, max_depth=5, min_child_weight=3, gamma=0.3, colsample_bytree=0.67, subsample=0.78, reg_alpha=0, reg_lambda=0</t>
   </si>
 </sst>
 </file>
@@ -487,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +522,7 @@
     <col min="3" max="3" width="24.42578125" customWidth="1"/>
     <col min="4" max="4" width="62.5703125" customWidth="1"/>
     <col min="5" max="5" width="28" style="2" customWidth="1"/>
-    <col min="6" max="6" width="119" customWidth="1"/>
+    <col min="6" max="6" width="126.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -658,6 +682,12 @@
       <c r="D10" t="s">
         <v>19</v>
       </c>
+      <c r="E10" s="2">
+        <v>0.58615555555555499</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -726,6 +756,12 @@
       <c r="D14" t="s">
         <v>19</v>
       </c>
+      <c r="E14" s="2">
+        <v>0.67968333333333297</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -738,6 +774,12 @@
       <c r="D15" t="s">
         <v>19</v>
       </c>
+      <c r="E15" s="2">
+        <v>0.97416666666666596</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -776,6 +818,12 @@
       <c r="D18" t="s">
         <v>26</v>
       </c>
+      <c r="E18" s="2">
+        <v>0.59760000000000002</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -794,7 +842,7 @@
         <v>0.9163</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -812,7 +860,7 @@
         <v>0.62690000000000001</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -830,7 +878,7 @@
         <v>0.94850000000000001</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -844,6 +892,12 @@
       <c r="D22" t="s">
         <v>26</v>
       </c>
+      <c r="E22" s="2">
+        <v>0.6794</v>
+      </c>
+      <c r="F22" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -856,6 +910,12 @@
       <c r="D23" t="s">
         <v>26</v>
       </c>
+      <c r="E23" s="2">
+        <v>0.97340000000000004</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
@@ -868,6 +928,12 @@
       <c r="D24" t="s">
         <v>26</v>
       </c>
+      <c r="E24" s="2">
+        <v>0.76989300000000005</v>
+      </c>
+      <c r="F24" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -879,6 +945,12 @@
       </c>
       <c r="D25" t="s">
         <v>26</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.9819</v>
+      </c>
+      <c r="F25" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added model analysis graphs.
</commit_message>
<xml_diff>
--- a/model_analysis.xlsx
+++ b/model_analysis.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winst\OneDrive\BWSI piPACT\piPACT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/31a3af44735637da/BWSI piPACT/piPACT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733041A5-D202-4626-BF80-64DB7291C7AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F72DBB3-1A6B-477A-99D5-2582E632919A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="0" windowWidth="17280" windowHeight="10188" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -794,7 +795,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -903,7 +904,7 @@
                 </c:tx>
                 <c:spPr>
                   <a:solidFill>
-                    <a:schemeClr val="accent2"/>
+                    <a:schemeClr val="accent4"/>
                   </a:solidFill>
                   <a:ln>
                     <a:noFill/>
@@ -1228,7 +1229,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1337,7 +1338,7 @@
                 </c:tx>
                 <c:spPr>
                   <a:solidFill>
-                    <a:schemeClr val="accent2"/>
+                    <a:schemeClr val="accent4"/>
                   </a:solidFill>
                   <a:ln>
                     <a:noFill/>
@@ -1662,7 +1663,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1771,7 +1772,7 @@
                 </c:tx>
                 <c:spPr>
                   <a:solidFill>
-                    <a:schemeClr val="accent2"/>
+                    <a:schemeClr val="accent4"/>
                   </a:solidFill>
                   <a:ln>
                     <a:noFill/>
@@ -4272,7 +4273,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4360,7 +4361,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent4"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4694,7 +4695,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4803,7 +4804,7 @@
                 </c:tx>
                 <c:spPr>
                   <a:solidFill>
-                    <a:schemeClr val="accent2"/>
+                    <a:schemeClr val="accent4"/>
                   </a:solidFill>
                   <a:ln>
                     <a:noFill/>
@@ -5127,7 +5128,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -5236,7 +5237,7 @@
                 </c:tx>
                 <c:spPr>
                   <a:solidFill>
-                    <a:schemeClr val="accent2"/>
+                    <a:schemeClr val="accent4"/>
                   </a:solidFill>
                   <a:ln>
                     <a:noFill/>
@@ -5510,12 +5511,9 @@
 </file>
 
 <file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -5550,12 +5548,9 @@
 </file>
 
 <file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -5590,12 +5585,9 @@
 </file>
 
 <file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -5830,12 +5822,9 @@
 </file>
 
 <file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -5870,12 +5859,9 @@
 </file>
 
 <file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -5910,12 +5896,9 @@
 </file>
 
 <file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -12724,21 +12707,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="62.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="62.5546875" customWidth="1"/>
     <col min="5" max="5" width="28" style="2" customWidth="1"/>
-    <col min="6" max="6" width="126.7109375" customWidth="1"/>
+    <col min="6" max="6" width="126.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12758,7 +12741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -12778,7 +12761,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>56</v>
       </c>
@@ -12798,7 +12781,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>5</v>
@@ -12816,7 +12799,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>6</v>
@@ -12834,7 +12817,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>3</v>
@@ -12852,7 +12835,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>4</v>
@@ -12870,7 +12853,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>5</v>
@@ -12888,7 +12871,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>6</v>
@@ -12906,7 +12889,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -12926,7 +12909,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>56</v>
       </c>
@@ -12946,7 +12929,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
         <v>5</v>
@@ -12964,7 +12947,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>6</v>
@@ -12982,7 +12965,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
         <v>3</v>
@@ -13000,7 +12983,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
         <v>4</v>
@@ -13018,7 +13001,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
         <v>5</v>
@@ -13036,7 +13019,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
         <v>6</v>
@@ -13054,7 +13037,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -13074,7 +13057,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>56</v>
       </c>
@@ -13094,7 +13077,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" t="s">
         <v>5</v>
@@ -13112,7 +13095,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
         <v>6</v>
@@ -13130,7 +13113,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
         <v>3</v>
@@ -13148,7 +13131,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
         <v>4</v>
@@ -13166,7 +13149,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
         <v>5</v>
@@ -13184,7 +13167,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
         <v>6</v>
@@ -13202,7 +13185,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -13222,7 +13205,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
@@ -13242,7 +13225,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" t="s">
         <v>5</v>
@@ -13260,7 +13243,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" t="s">
         <v>6</v>
@@ -13278,7 +13261,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" t="s">
         <v>3</v>
@@ -13296,7 +13279,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" t="s">
         <v>4</v>
@@ -13314,7 +13297,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" t="s">
         <v>5</v>
@@ -13332,7 +13315,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" t="s">
         <v>6</v>
@@ -13350,7 +13333,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
@@ -13370,7 +13353,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>19</v>
       </c>
@@ -13390,7 +13373,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" t="s">
         <v>5</v>
@@ -13408,7 +13391,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" t="s">
         <v>6</v>
@@ -13426,7 +13409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" t="s">
         <v>3</v>
@@ -13444,7 +13427,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" t="s">
         <v>4</v>
@@ -13462,7 +13445,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" t="s">
         <v>5</v>
@@ -13480,7 +13463,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" t="s">
         <v>6</v>
@@ -13498,7 +13481,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>11</v>
       </c>
@@ -13518,7 +13501,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>56</v>
       </c>
@@ -13538,7 +13521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" t="s">
         <v>5</v>
@@ -13556,7 +13539,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" t="s">
         <v>6</v>
@@ -13574,7 +13557,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" t="s">
         <v>3</v>
@@ -13592,7 +13575,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" t="s">
         <v>4</v>
@@ -13610,7 +13593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" t="s">
         <v>5</v>
@@ -13628,7 +13611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" t="s">
         <v>6</v>

</xml_diff>